<commit_message>
modelito con el frame unico q se ve vacilon
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -185,10 +185,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="133">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -658,7 +664,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="121">
+      <c r="A2" t="n" s="127">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -697,7 +703,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="123">
+      <c r="A3" t="n" s="129">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -736,7 +742,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="125">
+      <c r="A4" t="n" s="131">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">

</xml_diff>

<commit_message>
ya sirve agregar usuario :D
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -185,10 +185,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -664,7 +676,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="127">
+      <c r="A2" t="n" s="139">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -703,7 +715,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="129">
+      <c r="A3" t="n" s="141">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -742,7 +754,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="131">
+      <c r="A4" t="n" s="143">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">

</xml_diff>

<commit_message>
Ya sirve todo lo que sea las funciones del superusuario
mañana le pongo las imagenes
</commit_message>
<xml_diff>
--- a/IProyectoDiseño/src/files/DatosFormulario.xlsx
+++ b/IProyectoDiseño/src/files/DatosFormulario.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="38">
   <si>
     <t>Periodo</t>
   </si>
@@ -185,10 +185,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -676,7 +682,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="139">
+      <c r="A2" t="n" s="145">
         <v>42789.0</v>
       </c>
       <c r="B2" t="s">
@@ -715,7 +721,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n" s="141">
+      <c r="A3" t="n" s="147">
         <v>42825.0</v>
       </c>
       <c r="B3" t="s">
@@ -754,7 +760,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n" s="143">
+      <c r="A4" t="n" s="149">
         <v>43285.95474537037</v>
       </c>
       <c r="B4" t="s">

</xml_diff>